<commit_message>
works with basic test
</commit_message>
<xml_diff>
--- a/src/Tabelle.xlsx
+++ b/src/Tabelle.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600" activeTab="2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="84">
   <si>
     <t>è</t>
   </si>
@@ -226,9 +226,6 @@
     <t xml:space="preserve">div </t>
   </si>
   <si>
-    <t>mult, div , mod, open</t>
-  </si>
-  <si>
     <t>open, add, sub , identifier, numeral</t>
   </si>
   <si>
@@ -239,13 +236,46 @@
   </si>
   <si>
     <t>last</t>
+  </si>
+  <si>
+    <t>pow</t>
+  </si>
+  <si>
+    <t>mult pow</t>
+  </si>
+  <si>
+    <t>div pow</t>
+  </si>
+  <si>
+    <t>mod pow</t>
+  </si>
+  <si>
+    <t>pow term2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor pow2 </t>
+  </si>
+  <si>
+    <t>pow2</t>
+  </si>
+  <si>
+    <t>pot factor pow2</t>
+  </si>
+  <si>
+    <t>pot</t>
+  </si>
+  <si>
+    <t>mult, div , mod, open,semicolon</t>
+  </si>
+  <si>
+    <t>mult, div , mod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,7 +301,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,8 +368,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -362,11 +398,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -394,17 +441,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -478,6 +534,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -512,6 +569,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -687,20 +745,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -711,7 +769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -722,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -733,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -744,7 +802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -755,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -766,7 +824,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -777,7 +835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -788,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -799,7 +857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -810,7 +868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -821,7 +879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -832,7 +890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -843,7 +901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -854,7 +912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -865,7 +923,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -876,7 +934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -887,7 +945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -898,7 +956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -909,7 +967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -920,16 +978,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
   </sheetData>
@@ -939,14 +997,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -954,7 +1012,7 @@
     <col min="7" max="7" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
@@ -965,7 +1023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
@@ -976,7 +1034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>3</v>
       </c>
@@ -987,7 +1045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +1089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
@@ -1042,7 +1100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>26</v>
       </c>
@@ -1053,7 +1111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1134,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>46</v>
       </c>
@@ -1088,7 +1146,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>46</v>
       </c>
@@ -1099,7 +1157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>29</v>
       </c>
@@ -1110,7 +1168,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>29</v>
       </c>
@@ -1121,7 +1179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1190,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>60</v>
       </c>
@@ -1143,7 +1201,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>60</v>
       </c>
@@ -1154,7 +1212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>31</v>
       </c>
@@ -1165,7 +1223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>31</v>
       </c>
@@ -1176,7 +1234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +1246,7 @@
       </c>
       <c r="G21" s="26"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>19</v>
       </c>
@@ -1199,7 +1257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>19</v>
       </c>
@@ -1210,7 +1268,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>19</v>
       </c>
@@ -1221,7 +1279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>19</v>
       </c>
@@ -1232,7 +1290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1301,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
   </sheetData>
@@ -1252,14 +1310,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="3" max="3" width="51.140625" customWidth="1"/>
@@ -1267,15 +1325,15 @@
     <col min="5" max="5" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
@@ -1285,11 +1343,14 @@
       <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
@@ -1297,27 +1358,27 @@
         <v>0</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>3</v>
       </c>
@@ -1328,11 +1389,11 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1345,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>5</v>
       </c>
@@ -1359,7 +1420,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>26</v>
       </c>
@@ -1373,8 +1434,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1384,10 +1445,10 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>6</v>
       </c>
@@ -1398,10 +1459,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>11</v>
       </c>
@@ -1412,10 +1473,10 @@
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>46</v>
       </c>
@@ -1432,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>46</v>
       </c>
@@ -1446,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>29</v>
       </c>
@@ -1460,7 +1521,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>29</v>
       </c>
@@ -1474,7 +1535,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>14</v>
       </c>
@@ -1482,13 +1543,13 @@
         <v>0</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>60</v>
       </c>
@@ -1499,13 +1560,13 @@
         <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>60</v>
       </c>
@@ -1519,7 +1580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>31</v>
       </c>
@@ -1527,13 +1588,13 @@
         <v>0</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>31</v>
       </c>
@@ -1541,13 +1602,13 @@
         <v>0</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>31</v>
       </c>
@@ -1555,79 +1616,121 @@
         <v>0</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="24" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="B29" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="24" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="24" t="s">
+      <c r="B30" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D30" s="24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="24" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="24" t="s">
+      <c r="B31" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D31" s="24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="24" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="24" t="s">
+      <c r="B32" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D32" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="24" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="B33" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D33" s="24" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1637,14 +1740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F32"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
@@ -1654,7 +1757,7 @@
     <col min="6" max="6" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>36</v>
       </c>
@@ -1662,7 +1765,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
@@ -1679,7 +1782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1694,7 +1797,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1709,7 +1812,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1724,7 +1827,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1739,7 +1842,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +1857,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
@@ -1771,7 +1874,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>5</v>
       </c>
@@ -1788,7 +1891,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>26</v>
       </c>
@@ -1803,7 +1906,7 @@
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
@@ -1818,7 +1921,7 @@
       </c>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
@@ -1835,7 +1938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>11</v>
       </c>
@@ -1852,7 +1955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>46</v>
       </c>
@@ -1869,7 +1972,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1884,7 +1987,7 @@
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
         <v>29</v>
       </c>
@@ -1901,7 +2004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
         <v>29</v>
       </c>
@@ -1916,7 +2019,7 @@
       </c>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
         <v>14</v>
       </c>
@@ -1931,7 +2034,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
@@ -1946,7 +2049,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>31</v>
       </c>
@@ -1963,7 +2066,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>31</v>
       </c>
@@ -1978,7 +2081,7 @@
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>31</v>
       </c>
@@ -1993,7 +2096,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>35</v>
       </c>
@@ -2008,7 +2111,7 @@
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>19</v>
       </c>
@@ -2023,7 +2126,7 @@
       </c>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>19</v>
       </c>
@@ -2038,7 +2141,7 @@
       </c>
       <c r="F29" s="14"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>19</v>
       </c>
@@ -2053,7 +2156,7 @@
       </c>
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2171,7 @@
       </c>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>19</v>
       </c>

</xml_diff>